<commit_message>
add frontend demo view
</commit_message>
<xml_diff>
--- a/output/step4_interactive_filter/filtered_flights_query_1.xlsx
+++ b/output/step4_interactive_filter/filtered_flights_query_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,32 +498,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Turkish Airlines</t>
+          <t>LOT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3:30 pm</t>
+          <t>1:55 pm</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7:10 pm</t>
+          <t>8:20 pm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$836</t>
+          <t>$590</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>nonstop</t>
+          <t>1 stop (WAW)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10h 40m</t>
+          <t>13h 25m</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2025-04-16</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -558,37 +558,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Multiple airlines</t>
+          <t>LOT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4:30 pm</t>
+          <t>1:55 pm</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2:15 pm</t>
+          <t>8:20 pm</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$364</t>
+          <t>$558</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2 stops (OTP, DUB)</t>
+          <t>1 stop (WAW)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>28h 45m</t>
+          <t>13h 25m</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>SAW</t>
+          <t>IST</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2025-04-16</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -623,7 +623,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1:55 pm</t>
+          <t>11:25 am</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -633,17 +633,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$727</t>
+          <t>$568</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1 stop (WAW)</t>
+          <t>2 stops (KRK, WAW)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>13h 25m</t>
+          <t>15h 55m</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2025-04-16</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -678,32 +678,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Turkish Airlines</t>
+          <t>LOT</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3:30 pm</t>
+          <t>1:55 pm</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7:10 pm</t>
+          <t>8:20 pm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$981</t>
+          <t>$590</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>nonstop</t>
+          <t>1 stop (WAW)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10h 40m</t>
+          <t>13h 25m</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2025-04-21</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -738,32 +738,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Turkish Airlines</t>
+          <t>LOT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3:30 pm</t>
+          <t>1:55 pm</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7:10 pm</t>
+          <t>8:20 pm</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$836</t>
+          <t>$558</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>nonstop</t>
+          <t>1 stop (WAW)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10h 40m</t>
+          <t>13h 25m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2025-04-21</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -787,9 +787,69 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LOT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11:25 am</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8:20 pm</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$568</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2 stops (KRK, WAW)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>15h 55m</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>IST</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>YYZ</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-04-17</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>4</v>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>{}</t>
         </is>

</xml_diff>